<commit_message>
Framework ready with Reporting, ScreenShot, POM, PageFactory, Dynamic value
</commit_message>
<xml_diff>
--- a/src/main/java/com/agentaDemo/resource/ExcelData.xlsx
+++ b/src/main/java/com/agentaDemo/resource/ExcelData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87B403C-619F-4EE2-B1C5-1C9E4416A33E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5CE10E-53F2-47FD-9ED5-0252FB9AB712}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17670" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>Username</t>
   </si>
@@ -42,9 +42,6 @@
     <t>https://localhost:8080/</t>
   </si>
   <si>
-    <t>749932</t>
-  </si>
-  <si>
     <t>123456</t>
   </si>
   <si>
@@ -81,19 +78,22 @@
     <t>ext_ch2</t>
   </si>
   <si>
-    <t>749937</t>
-  </si>
-  <si>
-    <t>749934</t>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>749936</t>
+  </si>
+  <si>
+    <t>749933</t>
+  </si>
+  <si>
+    <t>749939</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,10 +169,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -493,20 +491,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
@@ -514,134 +512,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="L6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="5" t="s">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="L9" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="L6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="2"/>
-      <c r="I8" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{E7D9946C-06BB-4D40-B46C-EC70E170F24E}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{40C338ED-A5D3-4696-9773-6E6CF0FF45AD}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{7D2DD646-61D7-4685-8F3F-0DFC8046B0E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated framework and test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/agentaDemo/resource/ExcelData.xlsx
+++ b/src/main/java/com/agentaDemo/resource/ExcelData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5CE10E-53F2-47FD-9ED5-0252FB9AB712}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C155EBE-5474-415C-AB2B-6BC240E01AC6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17670" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgentaTest" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Scenario</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>123456</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -78,16 +72,49 @@
     <t>ext_ch2</t>
   </si>
   <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>749936</t>
+    <t>749932</t>
+  </si>
+  <si>
+    <t>counsultAgent1</t>
+  </si>
+  <si>
+    <t>consultAgent2</t>
   </si>
   <si>
     <t>749933</t>
   </si>
   <si>
-    <t>749939</t>
+    <t>conference</t>
+  </si>
+  <si>
+    <t>Wrapupreasoncode</t>
+  </si>
+  <si>
+    <t>Wrap-Up Reason</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>LoginLogout</t>
+  </si>
+  <si>
+    <t>SignOutReason</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>signoutreasonChrome</t>
+  </si>
+  <si>
+    <t>signoutreasonFF</t>
+  </si>
+  <si>
+    <t>749931</t>
+  </si>
+  <si>
+    <t>signoutreasondriver</t>
   </si>
 </sst>
 </file>
@@ -491,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,19 +531,25 @@
     <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -527,182 +560,223 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F3" s="2" t="s">
-        <v>3</v>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="L5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="L6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="3" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="L9" s="2" t="s">
-        <v>18</v>
+      <c r="M9" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>